<commit_message>
updated Gantt charts, finished all points listed in #18 apart for the obvious one
</commit_message>
<xml_diff>
--- a/Compute.Documents/Gantt/Trimester 1.xlsx
+++ b/Compute.Documents/Gantt/Trimester 1.xlsx
@@ -145,9 +145,6 @@
     <t xml:space="preserve"> Period Highlight:</t>
   </si>
   <si>
-    <t>Honours Project</t>
-  </si>
-  <si>
     <t>Embed V8 Version 5.5.5</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>Debugging &amp; Testing</t>
+  </si>
+  <si>
+    <t>Trimester 1</t>
   </si>
 </sst>
 </file>
@@ -893,15 +893,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:AX40"/>
+  <dimension ref="B1:AX40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="BJ20" sqref="BJ20"/>
+      <selection activeCell="BB10" sqref="BB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="1" max="1" width="7.875" customWidth="1"/>
     <col min="2" max="2" width="36.375" style="2" customWidth="1"/>
     <col min="3" max="5" width="7.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.375" style="1" customWidth="1"/>
@@ -910,9 +910,10 @@
     <col min="9" max="28" width="2.75" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:50" ht="38.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:50" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -1087,7 +1088,7 @@
     </row>
     <row r="9" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="16">
         <v>1</v>
@@ -1114,7 +1115,7 @@
     </row>
     <row r="10" spans="2:50" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="16">
         <v>3</v>
@@ -1141,7 +1142,7 @@
     </row>
     <row r="11" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="16">
         <v>5</v>
@@ -1168,7 +1169,7 @@
     </row>
     <row r="12" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="16">
         <v>5</v>
@@ -1195,7 +1196,7 @@
     </row>
     <row r="13" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="16">
         <v>3</v>
@@ -1222,7 +1223,7 @@
     </row>
     <row r="14" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="16">
         <v>2</v>
@@ -1249,7 +1250,7 @@
     </row>
     <row r="15" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="16">
         <v>7</v>
@@ -1276,7 +1277,7 @@
     </row>
     <row r="16" spans="2:50" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="16">
         <v>12</v>
@@ -1303,7 +1304,7 @@
     </row>
     <row r="17" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="16">
         <v>9</v>
@@ -1330,7 +1331,7 @@
     </row>
     <row r="18" spans="2:28" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="16">
         <v>1</v>

</xml_diff>